<commit_message>
fix(python): Ensure `read_excel` and `read_ods` return identical frames across all engines when given empty spreadsheet tables
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/empty.xlsx
+++ b/py-polars/tests/unit/io/files/empty.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33C9C33B-0D7B-E046-9283-7C14FD77A285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AE8D4CF-F08A-644A-96CD-89AE387B4C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="12600" windowWidth="28040" windowHeight="17440" xr2:uid="{2E4FE14B-E712-4D4B-B323-91C9F4BA5C80}"/>
+    <workbookView xWindow="29500" yWindow="16300" windowWidth="28040" windowHeight="17440" xr2:uid="{2E4FE14B-E712-4D4B-B323-91C9F4BA5C80}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="no_data" sheetId="1" r:id="rId1"/>
+    <sheet name="no_rows" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,10 +36,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>colx</t>
+  </si>
+  <si>
+    <t>coly</t>
+  </si>
+  <si>
+    <t>colz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -86,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -126,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -232,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -374,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,4 +417,30 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K737373 Classification: Public</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A61C921-4CA4-2047-B6A5-B78AFFCFAEB1}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix(python): Ensure `read_excel` and `read_ods` return identical frames across all engines when given empty spreadsheet tables (#16802)
</commit_message>
<xml_diff>
--- a/py-polars/tests/unit/io/files/empty.xlsx
+++ b/py-polars/tests/unit/io/files/empty.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a13107q/PycharmProjects/polars/py-polars/tests/unit/io/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33C9C33B-0D7B-E046-9283-7C14FD77A285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AE8D4CF-F08A-644A-96CD-89AE387B4C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24380" yWindow="12600" windowWidth="28040" windowHeight="17440" xr2:uid="{2E4FE14B-E712-4D4B-B323-91C9F4BA5C80}"/>
+    <workbookView xWindow="29500" yWindow="16300" windowWidth="28040" windowHeight="17440" xr2:uid="{2E4FE14B-E712-4D4B-B323-91C9F4BA5C80}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="no_data" sheetId="1" r:id="rId1"/>
+    <sheet name="no_rows" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,10 +36,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>colx</t>
+  </si>
+  <si>
+    <t>coly</t>
+  </si>
+  <si>
+    <t>colz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -86,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -126,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -232,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -374,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -393,4 +417,30 @@
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K737373 Classification: Public</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A61C921-4CA4-2047-B6A5-B78AFFCFAEB1}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>